<commit_message>
Feat:It was separated by classes, it was tested that it would work with both divs and tables
</commit_message>
<xml_diff>
--- a/excels/ciudadPaises.xlsx
+++ b/excels/ciudadPaises.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,743 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Office</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Start date</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Airi Satou</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Accountant</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>27/11/2008</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Angelica Ramos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Chief Executive Officer (CEO)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>8/10/2009</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ashton Cox</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Junior Technical Author</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>11/1/2009</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Bradley Greer</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>12/10/2012</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Brenden Wagner</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>6/6/2011</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Brielle Williamson</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Integration Specialist</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>1/12/2012</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bruno Nash</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2/5/2011</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Caesar Vance</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Pre-Sales Support</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>11/12/2011</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cara Stevens</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sales Assistant</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5/12/2011</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Cedric Kelly</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Senior Javascript Developer</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Edinburgh</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>28/3/2012</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Charde Marshall</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Regional Director</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>15/10/2008</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Colleen Hurst</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Javascript Developer</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>14/9/2009</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dai Rios</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Personnel Lead</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Edinburgh</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>25/9/2012</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Donna Snider</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Customer Support</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>24/1/2011</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Doris Wilder</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Sales Assistant</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sydney</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>19/9/2010</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Finn Camacho</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Support Engineer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>6/7/2009</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Fiona Green</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Chief Operating Officer (COO)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10/3/2010</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Garrett Winters</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Accountant</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>24/7/2011</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Gavin Cortez</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Team Leader</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>25/10/2008</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Gavin Joyce</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Developer</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Edinburgh</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>21/12/2010</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Gloria Little</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Systems Administrator</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>New York</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>9/4/2009</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Haley Kennedy</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Senior Marketing Designer</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>17/12/2012</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Hermione Butler</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Regional Director</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>London</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>20/3/2011</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Herrod Chandler</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Sales Assistant</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>5/8/2012</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Hope Fuentes</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Secretary</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>San Francisco</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>11/2/2010</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>